<commit_message>
Working Version Before extra data download buttn
Mostly working version before adding data download button - download report still needs to be fixed
</commit_message>
<xml_diff>
--- a/www/ECHO_CST_Xwalk.xlsx
+++ b/www/ECHO_CST_Xwalk.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/fisher_adam_epa_gov/Documents/Projects/Clean Water Regulatory Branch/NPDES Section/RPA Tool/RPA app/www/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="258" documentId="8_{21D50573-512A-4502-8B8D-3CDB7753D21B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{647BDFD7-218E-40F1-9840-48A88649775B}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{1366E9CF-3013-4613-8E51-ED6759BF8286}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9AAE1B3F-CBFA-4879-B076-AF31993E2311}"/>
   <bookViews>
-    <workbookView xWindow="-33017" yWindow="-1894" windowWidth="33120" windowHeight="18000" xr2:uid="{2EB36A63-3E86-4DB7-9075-3CF9575CABFD}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="16663" windowHeight="8743" xr2:uid="{2EB36A63-3E86-4DB7-9075-3CF9575CABFD}"/>
   </bookViews>
   <sheets>
     <sheet name="ECHO_CST_Xwalk" sheetId="1" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="303">
   <si>
     <t>zinc</t>
   </si>
@@ -965,6 +965,9 @@
   </si>
   <si>
     <t>Radiation, gross beta</t>
+  </si>
+  <si>
+    <t>MISSING</t>
   </si>
   <si>
     <t>POLLUTANT_CODE</t>
@@ -1333,8 +1336,8 @@
   <dimension ref="A1:E150"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
+      <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.45" x14ac:dyDescent="0.5"/>
@@ -1347,7 +1350,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="B1" t="s">
         <v>269</v>
@@ -2895,11 +2898,11 @@
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A111" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="B111" t="e">
-        <v>#N/A</v>
+      <c r="A111">
+        <v>999999</v>
+      </c>
+      <c r="B111" t="s">
+        <v>301</v>
       </c>
       <c r="C111">
         <v>787</v>

</xml_diff>

<commit_message>
mods to Report, server, and ui, and ECHO_CST_Xwalk file
</commit_message>
<xml_diff>
--- a/www/ECHO_CST_Xwalk.xlsx
+++ b/www/ECHO_CST_Xwalk.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/fisher_adam_epa_gov/Documents/Projects/Clean Water Regulatory Branch/NPDES Section/RPA Tool/RPA app/www/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{1366E9CF-3013-4613-8E51-ED6759BF8286}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9AAE1B3F-CBFA-4879-B076-AF31993E2311}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="13_ncr:1_{1366E9CF-3013-4613-8E51-ED6759BF8286}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E1CD63E9-4B14-4FF4-8073-0DCA21E39BC2}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="16663" windowHeight="8743" xr2:uid="{2EB36A63-3E86-4DB7-9075-3CF9575CABFD}"/>
+    <workbookView xWindow="28680" yWindow="-1470" windowWidth="29040" windowHeight="15720" xr2:uid="{2EB36A63-3E86-4DB7-9075-3CF9575CABFD}"/>
   </bookViews>
   <sheets>
     <sheet name="ECHO_CST_Xwalk" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ECHO_CST_Xwalk!$A$1:$E$150</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ECHO_CST_Xwalk!$A$1:$E$151</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="308">
   <si>
     <t>zinc</t>
   </si>
@@ -971,6 +971,21 @@
   </si>
   <si>
     <t>POLLUTANT_CODE</t>
+  </si>
+  <si>
+    <t>NOTES</t>
+  </si>
+  <si>
+    <t>chromium</t>
+  </si>
+  <si>
+    <t>Chromium</t>
+  </si>
+  <si>
+    <t>Endosulfan, total</t>
+  </si>
+  <si>
+    <t>endosulfan</t>
   </si>
 </sst>
 </file>
@@ -1032,14 +1047,10 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1077,7 +1088,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1183,7 +1194,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1325,7 +1336,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1333,11 +1344,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83C15749-1197-4F70-9BE3-3617FA7DC270}">
-  <dimension ref="A1:E150"/>
+  <dimension ref="A1:E152"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A131" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G159" sqref="G159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.45" x14ac:dyDescent="0.5"/>
@@ -1348,7 +1359,7 @@
     <col min="4" max="4" width="37.8203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>302</v>
       </c>
@@ -1361,8 +1372,11 @@
       <c r="D1" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="E1" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A2">
         <v>10256</v>
       </c>
@@ -1376,7 +1390,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A3">
         <v>10257</v>
       </c>
@@ -1390,7 +1404,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A4">
         <v>10258</v>
       </c>
@@ -1404,7 +1418,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A5">
         <v>10278</v>
       </c>
@@ -1418,7 +1432,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A6">
         <v>10906</v>
       </c>
@@ -1432,7 +1446,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A7">
         <v>10130</v>
       </c>
@@ -1446,7 +1460,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A8">
         <v>10133</v>
       </c>
@@ -1460,7 +1474,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A9">
         <v>10262</v>
       </c>
@@ -1474,7 +1488,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A10">
         <v>10417</v>
       </c>
@@ -1488,7 +1502,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A11">
         <v>11399</v>
       </c>
@@ -1502,7 +1516,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A12">
         <v>10136</v>
       </c>
@@ -1516,7 +1530,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A13">
         <v>10031</v>
       </c>
@@ -1530,7 +1544,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A14">
         <v>10140</v>
       </c>
@@ -1544,7 +1558,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A15">
         <v>10239</v>
       </c>
@@ -1558,7 +1572,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A16">
         <v>10380</v>
       </c>
@@ -2241,1236 +2255,1267 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A64">
-        <v>1055</v>
+        <v>1012</v>
       </c>
       <c r="B64" t="s">
-        <v>209</v>
+        <v>305</v>
       </c>
       <c r="C64">
-        <v>274</v>
+        <v>180</v>
       </c>
       <c r="D64" t="s">
-        <v>86</v>
+        <v>304</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A65">
-        <v>11106</v>
+        <v>1055</v>
       </c>
       <c r="B65" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C65">
-        <v>149</v>
+        <v>274</v>
       </c>
       <c r="D65" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A66">
-        <v>1165</v>
+        <v>11106</v>
       </c>
       <c r="B66" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C66">
-        <v>521</v>
+        <v>149</v>
       </c>
       <c r="D66" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A67">
-        <v>5123</v>
+        <v>1165</v>
       </c>
       <c r="B67" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C67">
-        <v>137</v>
+        <v>521</v>
       </c>
       <c r="D67" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A68">
-        <v>12080</v>
+        <v>5123</v>
       </c>
       <c r="B68" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C68">
-        <v>16</v>
+        <v>137</v>
       </c>
       <c r="D68" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A69">
-        <v>10408</v>
+        <v>12080</v>
       </c>
       <c r="B69" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C69">
-        <v>531</v>
+        <v>16</v>
       </c>
       <c r="D69" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A70">
-        <v>10238</v>
+        <v>10408</v>
       </c>
       <c r="B70" t="s">
-        <v>271</v>
+        <v>214</v>
       </c>
       <c r="C70">
-        <v>654</v>
+        <v>531</v>
       </c>
       <c r="D70" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A71">
-        <v>11660</v>
+        <v>10238</v>
       </c>
       <c r="B71" t="s">
-        <v>215</v>
+        <v>271</v>
       </c>
       <c r="C71">
-        <v>276</v>
+        <v>654</v>
       </c>
       <c r="D71" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A72">
-        <v>10039</v>
+        <v>11660</v>
       </c>
       <c r="B72" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C72">
-        <v>138</v>
+        <v>276</v>
       </c>
       <c r="D72" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A73">
-        <v>10008</v>
+        <v>10039</v>
       </c>
       <c r="B73" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C73">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D73" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A74">
-        <v>10631</v>
+        <v>10008</v>
       </c>
       <c r="B74" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C74">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D74" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A75">
-        <v>10007</v>
+        <v>10631</v>
       </c>
       <c r="B75" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C75">
-        <v>536</v>
+        <v>140</v>
       </c>
       <c r="D75" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A76">
-        <v>3051</v>
+        <v>10007</v>
       </c>
       <c r="B76" t="s">
-        <v>272</v>
+        <v>219</v>
       </c>
       <c r="C76">
-        <v>392</v>
+        <v>536</v>
       </c>
       <c r="D76" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A77">
-        <v>10756</v>
+        <v>3051</v>
       </c>
       <c r="B77" t="s">
-        <v>220</v>
+        <v>272</v>
       </c>
       <c r="C77">
-        <v>655</v>
+        <v>392</v>
       </c>
       <c r="D77" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A78">
-        <v>10040</v>
+        <v>10756</v>
       </c>
       <c r="B78" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C78">
-        <v>781</v>
+        <v>655</v>
       </c>
       <c r="D78" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A79">
-        <v>10627</v>
+        <v>10040</v>
       </c>
       <c r="B79" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C79">
-        <v>522</v>
+        <v>781</v>
       </c>
       <c r="D79" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A80">
-        <v>11237</v>
+        <v>10627</v>
       </c>
       <c r="B80" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C80">
-        <v>784</v>
+        <v>522</v>
       </c>
       <c r="D80" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A81">
-        <v>10157</v>
+        <v>11237</v>
       </c>
       <c r="B81" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C81">
-        <v>141</v>
+        <v>784</v>
       </c>
       <c r="D81" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A82">
-        <v>10287</v>
+        <v>10157</v>
       </c>
       <c r="B82" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C82">
-        <v>317</v>
+        <v>141</v>
       </c>
       <c r="D82" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A83">
-        <v>7822</v>
+        <v>10287</v>
       </c>
       <c r="B83" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C83">
-        <v>913</v>
+        <v>317</v>
       </c>
       <c r="D83" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A84">
-        <v>10072</v>
+        <v>7822</v>
       </c>
       <c r="B84" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C84">
-        <v>18</v>
+        <v>913</v>
       </c>
       <c r="D84" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A85">
-        <v>1822</v>
+        <v>10072</v>
       </c>
       <c r="B85" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C85">
-        <v>696</v>
+        <v>18</v>
       </c>
       <c r="D85" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A86">
-        <v>10228</v>
+        <v>1822</v>
       </c>
       <c r="B86" t="s">
-        <v>273</v>
+        <v>228</v>
       </c>
       <c r="C86">
-        <v>1041</v>
+        <v>696</v>
       </c>
       <c r="D86" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A87">
-        <v>10969</v>
+        <v>10228</v>
       </c>
       <c r="B87" t="s">
-        <v>300</v>
+        <v>273</v>
       </c>
       <c r="C87">
-        <v>597</v>
+        <v>1041</v>
       </c>
       <c r="D87" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A88">
-        <v>10406</v>
+        <v>10969</v>
       </c>
       <c r="B88" t="s">
-        <v>229</v>
+        <v>300</v>
       </c>
       <c r="C88">
-        <v>282</v>
+        <v>597</v>
       </c>
       <c r="D88" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A89">
-        <v>10748</v>
+        <v>10406</v>
       </c>
       <c r="B89" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C89">
-        <v>523</v>
+        <v>282</v>
       </c>
       <c r="D89" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A90">
-        <v>10716</v>
+        <v>10748</v>
       </c>
       <c r="B90" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C90">
-        <v>406</v>
+        <v>523</v>
       </c>
       <c r="D90" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A91">
-        <v>10159</v>
+        <v>10716</v>
       </c>
       <c r="B91" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C91">
-        <v>524</v>
+        <v>406</v>
       </c>
       <c r="D91" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A92">
-        <v>10017</v>
+        <v>10159</v>
       </c>
       <c r="B92" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C92">
-        <v>277</v>
+        <v>524</v>
       </c>
       <c r="D92" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A93">
-        <v>11128</v>
+        <v>10017</v>
       </c>
       <c r="B93" t="s">
-        <v>274</v>
+        <v>233</v>
       </c>
       <c r="C93">
-        <v>1053</v>
+        <v>277</v>
       </c>
       <c r="D93" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A94">
-        <v>10662</v>
+        <v>11128</v>
       </c>
       <c r="B94" t="s">
-        <v>234</v>
+        <v>274</v>
       </c>
       <c r="C94">
-        <v>783</v>
+        <v>1053</v>
       </c>
       <c r="D94" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A95">
-        <v>10266</v>
+        <v>10662</v>
       </c>
       <c r="B95" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C95">
-        <v>19</v>
+        <v>783</v>
       </c>
       <c r="D95" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A96">
-        <v>10313</v>
+        <v>10266</v>
       </c>
       <c r="B96" t="s">
-        <v>275</v>
+        <v>235</v>
       </c>
       <c r="C96">
-        <v>245</v>
+        <v>19</v>
       </c>
       <c r="D96" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A97">
-        <v>10042</v>
+        <v>10313</v>
       </c>
       <c r="B97" t="s">
-        <v>236</v>
+        <v>275</v>
       </c>
       <c r="C97">
-        <v>404</v>
+        <v>245</v>
       </c>
       <c r="D97" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A98">
-        <v>6562</v>
+        <v>10042</v>
       </c>
       <c r="B98" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C98">
-        <v>273</v>
+        <v>404</v>
       </c>
       <c r="D98" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A99">
-        <v>10992</v>
+        <v>6562</v>
       </c>
       <c r="B99" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C99">
-        <v>918</v>
+        <v>273</v>
       </c>
       <c r="D99" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A100">
-        <v>2448</v>
+        <v>10992</v>
       </c>
       <c r="B100" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C100">
-        <v>134</v>
+        <v>918</v>
       </c>
       <c r="D100" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A101">
-        <v>10899</v>
+        <v>2448</v>
       </c>
       <c r="B101" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C101">
-        <v>528</v>
+        <v>134</v>
       </c>
       <c r="D101" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A102">
-        <v>10337</v>
+        <v>10899</v>
       </c>
       <c r="B102" t="s">
-        <v>276</v>
+        <v>240</v>
       </c>
       <c r="C102">
-        <v>788</v>
+        <v>528</v>
       </c>
       <c r="D102" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A103">
-        <v>10475</v>
+        <v>10337</v>
       </c>
       <c r="B103" t="s">
-        <v>241</v>
+        <v>276</v>
       </c>
       <c r="C103">
-        <v>589</v>
+        <v>788</v>
       </c>
       <c r="D103" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A104">
-        <v>10340</v>
+        <v>10475</v>
       </c>
       <c r="B104" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C104">
-        <v>771</v>
+        <v>589</v>
       </c>
       <c r="D104" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A105">
-        <v>10014</v>
+        <v>10340</v>
       </c>
       <c r="B105" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C105">
-        <v>529</v>
+        <v>771</v>
       </c>
       <c r="D105" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A106">
-        <v>10151</v>
+        <v>10014</v>
       </c>
       <c r="B106" t="s">
-        <v>278</v>
+        <v>243</v>
       </c>
       <c r="C106">
-        <v>662</v>
+        <v>529</v>
       </c>
       <c r="D106" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A107">
-        <v>2741</v>
+        <v>10151</v>
       </c>
       <c r="B107" t="s">
-        <v>244</v>
+        <v>278</v>
       </c>
       <c r="C107">
-        <v>264</v>
+        <v>662</v>
       </c>
       <c r="D107" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A108">
-        <v>10354</v>
+        <v>2741</v>
       </c>
       <c r="B108" t="s">
-        <v>277</v>
+        <v>244</v>
       </c>
       <c r="C108">
-        <v>320</v>
+        <v>264</v>
       </c>
       <c r="D108" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A109">
-        <v>2806</v>
+        <v>10354</v>
       </c>
       <c r="B109" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C109">
-        <v>582</v>
+        <v>320</v>
       </c>
       <c r="D109" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A110">
-        <v>10164</v>
+        <v>2806</v>
       </c>
       <c r="B110" t="s">
-        <v>245</v>
+        <v>279</v>
       </c>
       <c r="C110">
-        <v>772</v>
+        <v>582</v>
       </c>
       <c r="D110" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A111">
-        <v>999999</v>
+        <v>10164</v>
       </c>
       <c r="B111" t="s">
-        <v>301</v>
+        <v>245</v>
       </c>
       <c r="C111">
-        <v>787</v>
+        <v>772</v>
       </c>
       <c r="D111" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A112">
-        <v>10677</v>
+        <v>999999</v>
       </c>
       <c r="B112" t="s">
-        <v>280</v>
+        <v>301</v>
       </c>
       <c r="C112">
-        <v>711</v>
+        <v>787</v>
       </c>
       <c r="D112" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A113">
-        <v>11246</v>
+        <v>10677</v>
       </c>
       <c r="B113" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C113">
-        <v>583</v>
+        <v>711</v>
       </c>
       <c r="D113" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A114">
-        <v>12166</v>
+        <v>11246</v>
       </c>
       <c r="B114" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C114">
-        <v>478</v>
+        <v>583</v>
       </c>
       <c r="D114" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A115">
-        <v>10335</v>
+        <v>12166</v>
       </c>
       <c r="B115" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C115">
-        <v>640</v>
+        <v>478</v>
       </c>
       <c r="D115" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A116">
-        <v>10689</v>
+        <v>10335</v>
       </c>
       <c r="B116" t="s">
-        <v>246</v>
+        <v>283</v>
       </c>
       <c r="C116">
-        <v>265</v>
+        <v>640</v>
       </c>
       <c r="D116" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A117">
-        <v>10121</v>
+        <v>10689</v>
       </c>
       <c r="B117" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C117">
-        <v>773</v>
+        <v>265</v>
       </c>
       <c r="D117" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A118">
-        <v>10395</v>
+        <v>10121</v>
       </c>
       <c r="B118" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C118">
-        <v>431</v>
+        <v>773</v>
       </c>
       <c r="D118" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A119">
-        <v>10126</v>
+        <v>10395</v>
       </c>
       <c r="B119" t="s">
-        <v>297</v>
+        <v>248</v>
       </c>
       <c r="C119">
-        <v>1043</v>
+        <v>431</v>
       </c>
       <c r="D119" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A120">
-        <v>10127</v>
+        <v>10126</v>
       </c>
       <c r="B120" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C120">
-        <v>1045</v>
+        <v>1043</v>
       </c>
       <c r="D120" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A121">
-        <v>10125</v>
+        <v>10127</v>
       </c>
       <c r="B121" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C121">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="D121" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A122">
-        <v>10407</v>
+        <v>10125</v>
       </c>
       <c r="B122" t="s">
-        <v>249</v>
+        <v>295</v>
       </c>
       <c r="C122">
-        <v>410</v>
+        <v>1046</v>
       </c>
       <c r="D122" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A123">
-        <v>10165</v>
+        <v>10407</v>
       </c>
       <c r="B123" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C123">
-        <v>281</v>
+        <v>410</v>
       </c>
       <c r="D123" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A124">
-        <v>10396</v>
+        <v>10165</v>
       </c>
       <c r="B124" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C124">
-        <v>20</v>
+        <v>281</v>
       </c>
       <c r="D124" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A125">
-        <v>10510</v>
+        <v>10396</v>
       </c>
       <c r="B125" t="s">
-        <v>284</v>
+        <v>251</v>
       </c>
       <c r="C125">
-        <v>258</v>
+        <v>20</v>
       </c>
       <c r="D125" t="s">
-        <v>25</v>
-      </c>
-      <c r="E125" t="s">
-        <v>162</v>
+        <v>26</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A126">
-        <v>3321</v>
+        <v>10510</v>
       </c>
       <c r="B126" t="s">
-        <v>252</v>
+        <v>284</v>
       </c>
       <c r="C126">
-        <v>657</v>
+        <v>258</v>
       </c>
       <c r="D126" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="E126" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A127">
-        <v>10001</v>
+        <v>3321</v>
       </c>
       <c r="B127" t="s">
-        <v>294</v>
+        <v>252</v>
       </c>
       <c r="C127">
-        <v>143</v>
+        <v>657</v>
       </c>
       <c r="D127" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A128">
-        <v>7829</v>
+        <v>10001</v>
       </c>
       <c r="B128" t="s">
-        <v>253</v>
+        <v>294</v>
       </c>
       <c r="C128">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D128" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A129">
-        <v>10430</v>
+        <v>7829</v>
       </c>
       <c r="B129" t="s">
-        <v>285</v>
+        <v>253</v>
       </c>
       <c r="C129">
-        <v>46</v>
+        <v>144</v>
       </c>
       <c r="D129" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A130">
-        <v>3666</v>
+        <v>10430</v>
       </c>
       <c r="B130" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C130">
-        <v>658</v>
+        <v>46</v>
       </c>
       <c r="D130" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A131">
-        <v>3714</v>
+        <v>3666</v>
       </c>
       <c r="B131" t="s">
-        <v>254</v>
+        <v>286</v>
       </c>
       <c r="C131">
-        <v>13</v>
+        <v>658</v>
       </c>
       <c r="D131" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A132">
-        <v>112285</v>
+        <v>3714</v>
       </c>
       <c r="B132" t="s">
-        <v>287</v>
+        <v>254</v>
       </c>
       <c r="C132">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="D132" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A133">
-        <v>6101</v>
+        <v>112285</v>
       </c>
       <c r="B133" t="s">
-        <v>255</v>
+        <v>287</v>
       </c>
       <c r="C133">
-        <v>896</v>
+        <v>41</v>
       </c>
       <c r="D133" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A134">
-        <v>6106</v>
+        <v>6101</v>
       </c>
       <c r="B134" t="s">
-        <v>288</v>
+        <v>255</v>
       </c>
       <c r="C134">
-        <v>606</v>
+        <v>896</v>
       </c>
       <c r="D134" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A135">
-        <v>6128</v>
+        <v>6106</v>
       </c>
       <c r="B135" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C135">
-        <v>417</v>
+        <v>606</v>
       </c>
       <c r="D135" t="s">
-        <v>15</v>
-      </c>
-      <c r="E135" t="s">
-        <v>162</v>
+        <v>16</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A136">
-        <v>10284</v>
+        <v>6128</v>
       </c>
       <c r="B136" t="s">
-        <v>256</v>
+        <v>289</v>
       </c>
       <c r="C136">
-        <v>647</v>
+        <v>417</v>
       </c>
       <c r="D136" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="E136" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A137">
-        <v>4068</v>
+        <v>10284</v>
       </c>
       <c r="B137" t="s">
-        <v>290</v>
+        <v>256</v>
       </c>
       <c r="C137">
-        <v>403</v>
+        <v>647</v>
       </c>
       <c r="D137" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A138">
-        <v>10161</v>
+        <v>4068</v>
       </c>
       <c r="B138" t="s">
-        <v>257</v>
+        <v>290</v>
       </c>
       <c r="C138">
-        <v>648</v>
+        <v>403</v>
       </c>
       <c r="D138" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A139">
-        <v>375</v>
+        <v>10161</v>
       </c>
       <c r="B139" t="s">
-        <v>291</v>
+        <v>257</v>
       </c>
       <c r="C139">
-        <v>1321</v>
+        <v>648</v>
       </c>
       <c r="D139" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A140">
-        <v>4151</v>
+        <v>375</v>
       </c>
       <c r="B140" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C140">
-        <v>418</v>
+        <v>1321</v>
       </c>
       <c r="D140" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A141">
-        <v>2817</v>
+        <v>4151</v>
       </c>
       <c r="B141" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C141">
-        <v>961</v>
+        <v>418</v>
       </c>
       <c r="D141" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A142">
-        <v>5889</v>
+        <v>2817</v>
       </c>
       <c r="B142" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="C142">
-        <v>152</v>
+        <v>961</v>
       </c>
       <c r="D142" t="s">
-        <v>8</v>
-      </c>
-      <c r="E142" t="s">
-        <v>162</v>
+        <v>9</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A143">
-        <v>4234</v>
+        <v>5889</v>
       </c>
       <c r="B143" t="s">
-        <v>258</v>
+        <v>299</v>
       </c>
       <c r="C143">
-        <v>132</v>
+        <v>152</v>
       </c>
       <c r="D143" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="E143" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A144">
-        <v>10280</v>
+        <v>4234</v>
       </c>
       <c r="B144" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C144">
-        <v>45</v>
+        <v>132</v>
       </c>
       <c r="D144" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A145">
-        <v>12269</v>
+        <v>10280</v>
       </c>
       <c r="B145" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
       <c r="C145">
-        <v>154</v>
+        <v>45</v>
       </c>
       <c r="D145" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A146">
-        <v>10285</v>
+        <v>12269</v>
       </c>
       <c r="B146" t="s">
-        <v>260</v>
+        <v>268</v>
       </c>
       <c r="C146">
-        <v>197</v>
+        <v>154</v>
       </c>
       <c r="D146" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A147">
-        <v>10489</v>
+        <v>10285</v>
       </c>
       <c r="B147" t="s">
-        <v>298</v>
+        <v>260</v>
       </c>
       <c r="C147">
-        <v>305</v>
+        <v>197</v>
       </c>
       <c r="D147" t="s">
-        <v>3</v>
-      </c>
-      <c r="E147" t="s">
-        <v>162</v>
+        <v>4</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A148">
-        <v>6638</v>
+        <v>10489</v>
       </c>
       <c r="B148" t="s">
-        <v>261</v>
+        <v>298</v>
       </c>
       <c r="C148">
-        <v>292</v>
+        <v>305</v>
       </c>
       <c r="D148" t="s">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="E148" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A149">
-        <v>10282</v>
+        <v>6638</v>
       </c>
       <c r="B149" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C149">
-        <v>649</v>
+        <v>292</v>
       </c>
       <c r="D149" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A150">
+        <v>10282</v>
+      </c>
+      <c r="B150" t="s">
+        <v>262</v>
+      </c>
+      <c r="C150">
+        <v>649</v>
+      </c>
+      <c r="D150" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A151">
         <v>6352</v>
       </c>
-      <c r="B150" t="s">
+      <c r="B151" t="s">
         <v>263</v>
       </c>
-      <c r="C150">
+      <c r="C151">
         <v>650</v>
       </c>
-      <c r="D150" t="s">
+      <c r="D151" t="s">
         <v>0</v>
       </c>
     </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A152">
+        <v>10757</v>
+      </c>
+      <c r="B152" t="s">
+        <v>306</v>
+      </c>
+      <c r="C152">
+        <v>807</v>
+      </c>
+      <c r="D152" t="s">
+        <v>307</v>
+      </c>
+      <c r="E152" t="s">
+        <v>162</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:E150" xr:uid="{83C15749-1197-4F70-9BE3-3617FA7DC270}"/>
+  <autoFilter ref="A1:E151" xr:uid="{83C15749-1197-4F70-9BE3-3617FA7DC270}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
adding echo file & note about changing read funct.
</commit_message>
<xml_diff>
--- a/www/ECHO_CST_Xwalk.xlsx
+++ b/www/ECHO_CST_Xwalk.xlsx
@@ -3519,4 +3519,515 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004AFBD178B4236A4A9BE91A23126B4CB2" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="23985145a7a46d2ed41ebe5096764260">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xmlns:ns3="http://schemas.microsoft.com/sharepoint.v3" xmlns:ns4="http://schemas.microsoft.com/sharepoint/v3/fields" xmlns:ns5="bdd67f5a-0be2-4509-8207-0a269473728d" xmlns:ns6="f275cc5f-0233-4274-b569-dca1bec93dbb" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2469e46f73a3bcf44179adca5519bfd5" ns1:_="" ns2:_="" ns3:_="" ns4:_="" ns5:_="" ns6:_="">
+    <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
+    <xsd:import namespace="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4"/>
+    <xsd:import namespace="http://schemas.microsoft.com/sharepoint.v3"/>
+    <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3/fields"/>
+    <xsd:import namespace="bdd67f5a-0be2-4509-8207-0a269473728d"/>
+    <xsd:import namespace="f275cc5f-0233-4274-b569-dca1bec93dbb"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:Document_x0020_Creation_x0020_Date" minOccurs="0"/>
+                <xsd:element ref="ns2:Creator" minOccurs="0"/>
+                <xsd:element ref="ns2:EPA_x0020_Office" minOccurs="0"/>
+                <xsd:element ref="ns2:Record" minOccurs="0"/>
+                <xsd:element ref="ns3:CategoryDescription" minOccurs="0"/>
+                <xsd:element ref="ns2:Identifier" minOccurs="0"/>
+                <xsd:element ref="ns2:EPA_x0020_Contributor" minOccurs="0"/>
+                <xsd:element ref="ns2:External_x0020_Contributor" minOccurs="0"/>
+                <xsd:element ref="ns4:_Coverage" minOccurs="0"/>
+                <xsd:element ref="ns2:EPA_x0020_Related_x0020_Documents" minOccurs="0"/>
+                <xsd:element ref="ns4:_Source" minOccurs="0"/>
+                <xsd:element ref="ns2:Rights" minOccurs="0"/>
+                <xsd:element ref="ns1:Language" minOccurs="0"/>
+                <xsd:element ref="ns2:j747ac98061d40f0aa7bd47e1db5675d" minOccurs="0"/>
+                <xsd:element ref="ns2:TaxKeywordTaxHTField" minOccurs="0"/>
+                <xsd:element ref="ns2:TaxCatchAllLabel" minOccurs="0"/>
+                <xsd:element ref="ns2:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns5:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns5:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns6:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns6:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns5:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns5:MediaServiceSearchProperties" minOccurs="0"/>
+                <xsd:element ref="ns5:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns5:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns5:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns5:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns5:MediaServiceOCR" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="http://schemas.microsoft.com/sharepoint/v3" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="Language" ma:index="17" nillable="true" ma:displayName="Language" ma:default="English" ma:description="Select the document language from the drop down." ma:format="Dropdown" ma:internalName="Language" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Choice">
+          <xsd:enumeration value="Arabic (Saudi Arabia)"/>
+          <xsd:enumeration value="Bulgarian (Bulgaria)"/>
+          <xsd:enumeration value="Chinese (Hong Kong S.A.R.)"/>
+          <xsd:enumeration value="Chinese (People's Republic of China)"/>
+          <xsd:enumeration value="Chinese (Taiwan)"/>
+          <xsd:enumeration value="Croatian (Croatia)"/>
+          <xsd:enumeration value="Czech (Czech Republic)"/>
+          <xsd:enumeration value="Danish (Denmark)"/>
+          <xsd:enumeration value="Dutch (Netherlands)"/>
+          <xsd:enumeration value="English"/>
+          <xsd:enumeration value="Estonian (Estonia)"/>
+          <xsd:enumeration value="Finnish (Finland)"/>
+          <xsd:enumeration value="French (France)"/>
+          <xsd:enumeration value="German (Germany)"/>
+          <xsd:enumeration value="Greek (Greece)"/>
+          <xsd:enumeration value="Hebrew (Israel)"/>
+          <xsd:enumeration value="Hindi (India)"/>
+          <xsd:enumeration value="Hungarian (Hungary)"/>
+          <xsd:enumeration value="Indonesian (Indonesia)"/>
+          <xsd:enumeration value="Italian (Italy)"/>
+          <xsd:enumeration value="Japanese (Japan)"/>
+          <xsd:enumeration value="Korean (Korea)"/>
+          <xsd:enumeration value="Latvian (Latvia)"/>
+          <xsd:enumeration value="Lithuanian (Lithuania)"/>
+          <xsd:enumeration value="Malay (Malaysia)"/>
+          <xsd:enumeration value="Norwegian (Bokmal) (Norway)"/>
+          <xsd:enumeration value="Polish (Poland)"/>
+          <xsd:enumeration value="Portuguese (Brazil)"/>
+          <xsd:enumeration value="Portuguese (Portugal)"/>
+          <xsd:enumeration value="Romanian (Romania)"/>
+          <xsd:enumeration value="Russian (Russia)"/>
+          <xsd:enumeration value="Serbian (Latin) (Serbia)"/>
+          <xsd:enumeration value="Slovak (Slovakia)"/>
+          <xsd:enumeration value="Slovenian (Slovenia)"/>
+          <xsd:enumeration value="Spanish (Spain)"/>
+          <xsd:enumeration value="Swedish (Sweden)"/>
+          <xsd:enumeration value="Thai (Thailand)"/>
+          <xsd:enumeration value="Turkish (Turkey)"/>
+          <xsd:enumeration value="Ukrainian (Ukraine)"/>
+          <xsd:enumeration value="Urdu (Islamic Republic of Pakistan)"/>
+          <xsd:enumeration value="Vietnamese (Vietnam)"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="Document_x0020_Creation_x0020_Date" ma:index="2" nillable="true" ma:displayName="Document Date" ma:default="[today]" ma:description="Enter the date this document was last modified. The upload date has been entered by default." ma:format="DateOnly" ma:internalName="Document_x0020_Creation_x0020_Date" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:DateTime"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="Creator" ma:index="3" nillable="true" ma:displayName="Creator" ma:description="Enter the person primarily responsible for the document. The name of the person uploading the document has been entered by default." ma:list="UserInfo" ma:SharePointGroup="0" ma:internalName="Creator" ma:readOnly="false" ma:showField="ImnName">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:User">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="EPA_x0020_Office" ma:index="4" nillable="true" ma:displayName="EPA Office" ma:description="Enter the EPA organization primarily responsible for the document. The office of the person uploading the document has been entered by default." ma:internalName="EPA_x0020_Office" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="Record" ma:index="5" nillable="true" ma:displayName="Record" ma:default="Shared" ma:description="For documents that provide evidence of EPA decisions and actions, select &quot;Shared&quot; (open access) or &quot;Private&quot; (restricted access)." ma:format="Dropdown" ma:internalName="Record">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Choice">
+          <xsd:enumeration value="None"/>
+          <xsd:enumeration value="Shared"/>
+          <xsd:enumeration value="Private"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="Identifier" ma:index="9" nillable="true" ma:displayName="Identifier" ma:description="Enter all EPA identification numbers applicable to this document, one on each line." ma:internalName="Identifier" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="EPA_x0020_Contributor" ma:index="11" nillable="true" ma:displayName="EPA Contributor" ma:description="Enter an EPA person who contributed to the creation of the document but is not the primary author." ma:list="UserInfo" ma:SharePointGroup="0" ma:internalName="EPA_x0020_Contributor" ma:readOnly="false" ma:showField="ImnName">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:User">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="External_x0020_Contributor" ma:index="12" nillable="true" ma:displayName="External Contributor" ma:description="Enter a non-EPA person who contributed to the creation of the document but is not the primary author." ma:internalName="External_x0020_Contributor" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="EPA_x0020_Related_x0020_Documents" ma:index="14" nillable="true" ma:displayName="Other Related Documents" ma:description="Enter any related document." ma:internalName="EPA_x0020_Related_x0020_Documents" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="Rights" ma:index="16" nillable="true" ma:displayName="Rights" ma:description="Enter information about intellectual property rights held over the document (e.g. copyright, patent, trademark)." ma:internalName="Rights" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="j747ac98061d40f0aa7bd47e1db5675d" ma:index="19" nillable="true" ma:taxonomy="true" ma:internalName="j747ac98061d40f0aa7bd47e1db5675d" ma:taxonomyFieldName="Document_x0020_Type" ma:displayName="Document Type" ma:readOnly="false" ma:default="" ma:fieldId="{3747ac98-061d-40f0-aa7b-d47e1db5675d}" ma:sspId="29f62856-1543-49d4-a736-4569d363f533" ma:termSetId="e06cd6a9-a175-4da0-81cb-8dba7aa394ab" ma:anchorId="00000000-0000-0000-0000-000000000000" ma:open="false" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="TaxKeywordTaxHTField" ma:index="21" nillable="true" ma:taxonomy="true" ma:internalName="TaxKeywordTaxHTField" ma:taxonomyFieldName="TaxKeyword" ma:displayName="Enterprise Keywords" ma:readOnly="false" ma:fieldId="{23f27201-bee3-471e-b2e7-b64fd8b7ca38}" ma:taxonomyMulti="true" ma:sspId="29f62856-1543-49d4-a736-4569d363f533" ma:termSetId="00000000-0000-0000-0000-000000000000" ma:anchorId="00000000-0000-0000-0000-000000000000" ma:open="true" ma:isKeyword="true">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="TaxCatchAllLabel" ma:index="23" nillable="true" ma:displayName="Taxonomy Catch All Column1" ma:hidden="true" ma:list="{dbdac66b-d052-474f-b228-6e6894734c18}" ma:internalName="TaxCatchAllLabel" ma:readOnly="true" ma:showField="CatchAllDataLabel" ma:web="f275cc5f-0233-4274-b569-dca1bec93dbb">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="TaxCatchAll" ma:index="24" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{dbdac66b-d052-474f-b228-6e6894734c18}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="f275cc5f-0233-4274-b569-dca1bec93dbb">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="http://schemas.microsoft.com/sharepoint.v3" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="CategoryDescription" ma:index="6" nillable="true" ma:displayName="Description" ma:description="Enter a brief description." ma:internalName="CategoryDescription" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="http://schemas.microsoft.com/sharepoint/v3/fields" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="_Coverage" ma:index="13" nillable="true" ma:displayName="Coverage" ma:description="Enter the geographic location, jurisdiction, or time period for which the document is relevant." ma:internalName="_Coverage" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="_Source" ma:index="15" nillable="true" ma:displayName="Source" ma:description="Enter a source from which the document is derived." ma:internalName="_Source" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="bdd67f5a-0be2-4509-8207-0a269473728d" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="28" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="29" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="32" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="33" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="34" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="35" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="36" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="38" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="29f62856-1543-49d4-a736-4569d363f533" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="39" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="f275cc5f-0233-4274-b569-dca1bec93dbb" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="30" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="31" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="25" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="1" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="29f62856-1543-49d4-a736-4569d363f533" ContentTypeId="0x0101" PreviousValue="false"/>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_Source xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
+    <Language xmlns="http://schemas.microsoft.com/sharepoint/v3">English</Language>
+    <j747ac98061d40f0aa7bd47e1db5675d xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </j747ac98061d40f0aa7bd47e1db5675d>
+    <External_x0020_Contributor xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
+    <TaxKeywordTaxHTField xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </TaxKeywordTaxHTField>
+    <Record xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">Shared</Record>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="bdd67f5a-0be2-4509-8207-0a269473728d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <Rights xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
+    <Document_x0020_Creation_x0020_Date xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">2025-03-21T15:03:17+00:00</Document_x0020_Creation_x0020_Date>
+    <EPA_x0020_Office xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
+    <CategoryDescription xmlns="http://schemas.microsoft.com/sharepoint.v3" xsi:nil="true"/>
+    <Identifier xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
+    <_Coverage xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
+    <Creator xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Creator>
+    <EPA_x0020_Related_x0020_Documents xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
+    <EPA_x0020_Contributor xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </EPA_x0020_Contributor>
+    <TaxCatchAll xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F22E0A2-D0EC-4C7C-865F-DE6845FA3E9C}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{80008E65-ADEC-4216-A3A0-BEF3E3BB5FC4}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D8391EF2-9D7E-4327-9B91-14281F4F4FD4}"/>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{54B807D3-E722-4BD6-B9D1-3023D9D86526}"/>
 </file>
</xml_diff>

<commit_message>
adding REF_Parameter.csv file to www/ folder
</commit_message>
<xml_diff>
--- a/www/ECHO_CST_Xwalk.xlsx
+++ b/www/ECHO_CST_Xwalk.xlsx
@@ -3519,4 +3519,515 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004AFBD178B4236A4A9BE91A23126B4CB2" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="23985145a7a46d2ed41ebe5096764260">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xmlns:ns3="http://schemas.microsoft.com/sharepoint.v3" xmlns:ns4="http://schemas.microsoft.com/sharepoint/v3/fields" xmlns:ns5="bdd67f5a-0be2-4509-8207-0a269473728d" xmlns:ns6="f275cc5f-0233-4274-b569-dca1bec93dbb" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2469e46f73a3bcf44179adca5519bfd5" ns1:_="" ns2:_="" ns3:_="" ns4:_="" ns5:_="" ns6:_="">
+    <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
+    <xsd:import namespace="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4"/>
+    <xsd:import namespace="http://schemas.microsoft.com/sharepoint.v3"/>
+    <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3/fields"/>
+    <xsd:import namespace="bdd67f5a-0be2-4509-8207-0a269473728d"/>
+    <xsd:import namespace="f275cc5f-0233-4274-b569-dca1bec93dbb"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:Document_x0020_Creation_x0020_Date" minOccurs="0"/>
+                <xsd:element ref="ns2:Creator" minOccurs="0"/>
+                <xsd:element ref="ns2:EPA_x0020_Office" minOccurs="0"/>
+                <xsd:element ref="ns2:Record" minOccurs="0"/>
+                <xsd:element ref="ns3:CategoryDescription" minOccurs="0"/>
+                <xsd:element ref="ns2:Identifier" minOccurs="0"/>
+                <xsd:element ref="ns2:EPA_x0020_Contributor" minOccurs="0"/>
+                <xsd:element ref="ns2:External_x0020_Contributor" minOccurs="0"/>
+                <xsd:element ref="ns4:_Coverage" minOccurs="0"/>
+                <xsd:element ref="ns2:EPA_x0020_Related_x0020_Documents" minOccurs="0"/>
+                <xsd:element ref="ns4:_Source" minOccurs="0"/>
+                <xsd:element ref="ns2:Rights" minOccurs="0"/>
+                <xsd:element ref="ns1:Language" minOccurs="0"/>
+                <xsd:element ref="ns2:j747ac98061d40f0aa7bd47e1db5675d" minOccurs="0"/>
+                <xsd:element ref="ns2:TaxKeywordTaxHTField" minOccurs="0"/>
+                <xsd:element ref="ns2:TaxCatchAllLabel" minOccurs="0"/>
+                <xsd:element ref="ns2:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns5:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns5:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns6:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns6:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns5:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns5:MediaServiceSearchProperties" minOccurs="0"/>
+                <xsd:element ref="ns5:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns5:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns5:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns5:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns5:MediaServiceOCR" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="http://schemas.microsoft.com/sharepoint/v3" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="Language" ma:index="17" nillable="true" ma:displayName="Language" ma:default="English" ma:description="Select the document language from the drop down." ma:format="Dropdown" ma:internalName="Language" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Choice">
+          <xsd:enumeration value="Arabic (Saudi Arabia)"/>
+          <xsd:enumeration value="Bulgarian (Bulgaria)"/>
+          <xsd:enumeration value="Chinese (Hong Kong S.A.R.)"/>
+          <xsd:enumeration value="Chinese (People's Republic of China)"/>
+          <xsd:enumeration value="Chinese (Taiwan)"/>
+          <xsd:enumeration value="Croatian (Croatia)"/>
+          <xsd:enumeration value="Czech (Czech Republic)"/>
+          <xsd:enumeration value="Danish (Denmark)"/>
+          <xsd:enumeration value="Dutch (Netherlands)"/>
+          <xsd:enumeration value="English"/>
+          <xsd:enumeration value="Estonian (Estonia)"/>
+          <xsd:enumeration value="Finnish (Finland)"/>
+          <xsd:enumeration value="French (France)"/>
+          <xsd:enumeration value="German (Germany)"/>
+          <xsd:enumeration value="Greek (Greece)"/>
+          <xsd:enumeration value="Hebrew (Israel)"/>
+          <xsd:enumeration value="Hindi (India)"/>
+          <xsd:enumeration value="Hungarian (Hungary)"/>
+          <xsd:enumeration value="Indonesian (Indonesia)"/>
+          <xsd:enumeration value="Italian (Italy)"/>
+          <xsd:enumeration value="Japanese (Japan)"/>
+          <xsd:enumeration value="Korean (Korea)"/>
+          <xsd:enumeration value="Latvian (Latvia)"/>
+          <xsd:enumeration value="Lithuanian (Lithuania)"/>
+          <xsd:enumeration value="Malay (Malaysia)"/>
+          <xsd:enumeration value="Norwegian (Bokmal) (Norway)"/>
+          <xsd:enumeration value="Polish (Poland)"/>
+          <xsd:enumeration value="Portuguese (Brazil)"/>
+          <xsd:enumeration value="Portuguese (Portugal)"/>
+          <xsd:enumeration value="Romanian (Romania)"/>
+          <xsd:enumeration value="Russian (Russia)"/>
+          <xsd:enumeration value="Serbian (Latin) (Serbia)"/>
+          <xsd:enumeration value="Slovak (Slovakia)"/>
+          <xsd:enumeration value="Slovenian (Slovenia)"/>
+          <xsd:enumeration value="Spanish (Spain)"/>
+          <xsd:enumeration value="Swedish (Sweden)"/>
+          <xsd:enumeration value="Thai (Thailand)"/>
+          <xsd:enumeration value="Turkish (Turkey)"/>
+          <xsd:enumeration value="Ukrainian (Ukraine)"/>
+          <xsd:enumeration value="Urdu (Islamic Republic of Pakistan)"/>
+          <xsd:enumeration value="Vietnamese (Vietnam)"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="Document_x0020_Creation_x0020_Date" ma:index="2" nillable="true" ma:displayName="Document Date" ma:default="[today]" ma:description="Enter the date this document was last modified. The upload date has been entered by default." ma:format="DateOnly" ma:internalName="Document_x0020_Creation_x0020_Date" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:DateTime"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="Creator" ma:index="3" nillable="true" ma:displayName="Creator" ma:description="Enter the person primarily responsible for the document. The name of the person uploading the document has been entered by default." ma:list="UserInfo" ma:SharePointGroup="0" ma:internalName="Creator" ma:readOnly="false" ma:showField="ImnName">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:User">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="EPA_x0020_Office" ma:index="4" nillable="true" ma:displayName="EPA Office" ma:description="Enter the EPA organization primarily responsible for the document. The office of the person uploading the document has been entered by default." ma:internalName="EPA_x0020_Office" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="Record" ma:index="5" nillable="true" ma:displayName="Record" ma:default="Shared" ma:description="For documents that provide evidence of EPA decisions and actions, select &quot;Shared&quot; (open access) or &quot;Private&quot; (restricted access)." ma:format="Dropdown" ma:internalName="Record">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Choice">
+          <xsd:enumeration value="None"/>
+          <xsd:enumeration value="Shared"/>
+          <xsd:enumeration value="Private"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="Identifier" ma:index="9" nillable="true" ma:displayName="Identifier" ma:description="Enter all EPA identification numbers applicable to this document, one on each line." ma:internalName="Identifier" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="EPA_x0020_Contributor" ma:index="11" nillable="true" ma:displayName="EPA Contributor" ma:description="Enter an EPA person who contributed to the creation of the document but is not the primary author." ma:list="UserInfo" ma:SharePointGroup="0" ma:internalName="EPA_x0020_Contributor" ma:readOnly="false" ma:showField="ImnName">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:User">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="External_x0020_Contributor" ma:index="12" nillable="true" ma:displayName="External Contributor" ma:description="Enter a non-EPA person who contributed to the creation of the document but is not the primary author." ma:internalName="External_x0020_Contributor" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="EPA_x0020_Related_x0020_Documents" ma:index="14" nillable="true" ma:displayName="Other Related Documents" ma:description="Enter any related document." ma:internalName="EPA_x0020_Related_x0020_Documents" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="Rights" ma:index="16" nillable="true" ma:displayName="Rights" ma:description="Enter information about intellectual property rights held over the document (e.g. copyright, patent, trademark)." ma:internalName="Rights" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="j747ac98061d40f0aa7bd47e1db5675d" ma:index="19" nillable="true" ma:taxonomy="true" ma:internalName="j747ac98061d40f0aa7bd47e1db5675d" ma:taxonomyFieldName="Document_x0020_Type" ma:displayName="Document Type" ma:readOnly="false" ma:default="" ma:fieldId="{3747ac98-061d-40f0-aa7b-d47e1db5675d}" ma:sspId="29f62856-1543-49d4-a736-4569d363f533" ma:termSetId="e06cd6a9-a175-4da0-81cb-8dba7aa394ab" ma:anchorId="00000000-0000-0000-0000-000000000000" ma:open="false" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="TaxKeywordTaxHTField" ma:index="21" nillable="true" ma:taxonomy="true" ma:internalName="TaxKeywordTaxHTField" ma:taxonomyFieldName="TaxKeyword" ma:displayName="Enterprise Keywords" ma:readOnly="false" ma:fieldId="{23f27201-bee3-471e-b2e7-b64fd8b7ca38}" ma:taxonomyMulti="true" ma:sspId="29f62856-1543-49d4-a736-4569d363f533" ma:termSetId="00000000-0000-0000-0000-000000000000" ma:anchorId="00000000-0000-0000-0000-000000000000" ma:open="true" ma:isKeyword="true">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="TaxCatchAllLabel" ma:index="23" nillable="true" ma:displayName="Taxonomy Catch All Column1" ma:hidden="true" ma:list="{dbdac66b-d052-474f-b228-6e6894734c18}" ma:internalName="TaxCatchAllLabel" ma:readOnly="true" ma:showField="CatchAllDataLabel" ma:web="f275cc5f-0233-4274-b569-dca1bec93dbb">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="TaxCatchAll" ma:index="24" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{dbdac66b-d052-474f-b228-6e6894734c18}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="f275cc5f-0233-4274-b569-dca1bec93dbb">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="http://schemas.microsoft.com/sharepoint.v3" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="CategoryDescription" ma:index="6" nillable="true" ma:displayName="Description" ma:description="Enter a brief description." ma:internalName="CategoryDescription" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="http://schemas.microsoft.com/sharepoint/v3/fields" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="_Coverage" ma:index="13" nillable="true" ma:displayName="Coverage" ma:description="Enter the geographic location, jurisdiction, or time period for which the document is relevant." ma:internalName="_Coverage" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="_Source" ma:index="15" nillable="true" ma:displayName="Source" ma:description="Enter a source from which the document is derived." ma:internalName="_Source" ma:readOnly="false">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="bdd67f5a-0be2-4509-8207-0a269473728d" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="28" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="29" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="32" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="33" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="34" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="35" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="36" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="38" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="29f62856-1543-49d4-a736-4569d363f533" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="39" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="f275cc5f-0233-4274-b569-dca1bec93dbb" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="30" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="31" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="25" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="1" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="29f62856-1543-49d4-a736-4569d363f533" ContentTypeId="0x0101" PreviousValue="false"/>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_Source xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
+    <Language xmlns="http://schemas.microsoft.com/sharepoint/v3">English</Language>
+    <j747ac98061d40f0aa7bd47e1db5675d xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </j747ac98061d40f0aa7bd47e1db5675d>
+    <External_x0020_Contributor xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
+    <TaxKeywordTaxHTField xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </TaxKeywordTaxHTField>
+    <Record xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">Shared</Record>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="bdd67f5a-0be2-4509-8207-0a269473728d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <Rights xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
+    <Document_x0020_Creation_x0020_Date xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">2025-03-21T15:03:17+00:00</Document_x0020_Creation_x0020_Date>
+    <EPA_x0020_Office xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
+    <CategoryDescription xmlns="http://schemas.microsoft.com/sharepoint.v3" xsi:nil="true"/>
+    <Identifier xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
+    <_Coverage xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
+    <Creator xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Creator>
+    <EPA_x0020_Related_x0020_Documents xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
+    <EPA_x0020_Contributor xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </EPA_x0020_Contributor>
+    <TaxCatchAll xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F22E0A2-D0EC-4C7C-865F-DE6845FA3E9C}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{80008E65-ADEC-4216-A3A0-BEF3E3BB5FC4}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D8391EF2-9D7E-4327-9B91-14281F4F4FD4}"/>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{54B807D3-E722-4BD6-B9D1-3023D9D86526}"/>
 </file>
</xml_diff>